<commit_message>
modifies MCOs for 121 and 141
</commit_message>
<xml_diff>
--- a/121/CS 121 GenEd Outcome Correlation.xlsx
+++ b/121/CS 121 GenEd Outcome Correlation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chess/Documents/git-repos/scc-compsci/121/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{07AB0C3D-EC2A-5843-B37D-C872CA3A4B4A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{2FCBD4D0-5756-5743-B7A6-ADB4AA65A1D7}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27960" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-12280" yWindow="-19100" windowWidth="27940" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="102">
   <si>
     <t>Communication: Write effectively</t>
   </si>
@@ -329,6 +329,9 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>CS 121: Introduction to Programming</t>
   </si>
 </sst>
 </file>
@@ -367,7 +370,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -380,8 +383,14 @@
         <bgColor theme="4"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -404,11 +413,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -429,6 +475,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -542,8 +597,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="F2:I32" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="F2:I32" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="F3:I33" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="F3:I33" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Outcome From MCO" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Category" dataDxfId="2"/>
@@ -817,481 +872,546 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.5" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="11.5" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.1640625" style="8" customWidth="1"/>
+    <col min="1" max="1" width="11.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" style="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="66.83203125" style="1" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="32.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="0.1640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="7.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="6.83203125" style="1" customWidth="1"/>
     <col min="9" max="9" width="99.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="198" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:9" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="11"/>
+    </row>
+    <row r="2" spans="1:9" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C2" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="D1" s="6" t="s">
+      <c r="D2" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="3" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I3" s="4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="63" x14ac:dyDescent="0.25">
-      <c r="B3" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="F3" s="5" t="s">
+    <row r="4" spans="1:9" ht="84" x14ac:dyDescent="0.25">
+      <c r="C4" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="63" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>26</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>1</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="84" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>100</v>
+      </c>
       <c r="F5" s="5" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>1</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>61</v>
+        <v>27</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="84" hidden="1" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="84" x14ac:dyDescent="0.25">
+      <c r="B6" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>100</v>
+      </c>
       <c r="F6" s="5" t="s">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>1</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>2</v>
+        <v>61</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="63" hidden="1" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="84" hidden="1" x14ac:dyDescent="0.25">
       <c r="F7" s="5" t="s">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>1</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="63" hidden="1" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="84" hidden="1" x14ac:dyDescent="0.25">
       <c r="F8" s="5" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>1</v>
       </c>
       <c r="H8" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="84" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F9" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H9" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="I9" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="63" hidden="1" x14ac:dyDescent="0.25">
-      <c r="F9" s="5" t="s">
+    <row r="10" spans="1:9" ht="84" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F10" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="63" hidden="1" x14ac:dyDescent="0.25">
-      <c r="F10" s="5" t="s">
-        <v>32</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>17</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="63" hidden="1" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="84" hidden="1" x14ac:dyDescent="0.25">
       <c r="F11" s="5" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>17</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="63" hidden="1" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="84" hidden="1" x14ac:dyDescent="0.25">
       <c r="F12" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>17</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="63" hidden="1" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="84" hidden="1" x14ac:dyDescent="0.25">
       <c r="F13" s="5" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>17</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="63" hidden="1" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="84" hidden="1" x14ac:dyDescent="0.25">
       <c r="F14" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>17</v>
       </c>
       <c r="H14" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="84" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F15" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="I15" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="126" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="F15" s="5" t="s">
+    <row r="16" spans="1:9" ht="147" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="F16" s="5" t="s">
         <v>46</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="F16" s="5" t="s">
-        <v>49</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>47</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="126" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="147" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>100</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>47</v>
       </c>
       <c r="H17" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="147" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="H18" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="I17" s="2" t="s">
+      <c r="I18" s="2" t="s">
         <v>81</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="63" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="H18" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>100</v>
       </c>
+      <c r="B19" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>100</v>
+      </c>
       <c r="F19" s="5" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>4</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
-        <v>100</v>
-      </c>
       <c r="F20" s="5" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>4</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="63" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="B21" s="8" t="s">
         <v>100</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>4</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="F22" s="5" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="G22" s="5" t="s">
         <v>4</v>
       </c>
       <c r="H22" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F23" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H23" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="I22" s="2" t="s">
+      <c r="I23" s="2" t="s">
         <v>86</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="84" hidden="1" x14ac:dyDescent="0.25">
-      <c r="F23" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="G23" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H23" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="I23" s="2" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="126" hidden="1" x14ac:dyDescent="0.25">
       <c r="F24" s="5" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="G24" s="5" t="s">
         <v>9</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>29</v>
+        <v>55</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="84" hidden="1" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="126" hidden="1" x14ac:dyDescent="0.25">
       <c r="F25" s="5" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>9</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="84" hidden="1" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="126" hidden="1" x14ac:dyDescent="0.25">
       <c r="F26" s="5" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="G26" s="5" t="s">
         <v>9</v>
       </c>
       <c r="H26" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="126" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F27" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H27" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="I26" s="2" t="s">
+      <c r="I27" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="84" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="F27" s="5" t="s">
+    <row r="28" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="F28" s="5" t="s">
         <v>21</v>
-      </c>
-      <c r="G27" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H27" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I27" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="147" x14ac:dyDescent="0.25">
-      <c r="F28" s="5" t="s">
-        <v>44</v>
       </c>
       <c r="G28" s="5" t="s">
         <v>14</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="63" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="147" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>100</v>
+      </c>
       <c r="F29" s="5" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="G29" s="5" t="s">
         <v>14</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="63" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>100</v>
+      </c>
       <c r="F30" s="5" t="s">
-        <v>51</v>
+        <v>13</v>
       </c>
       <c r="G30" s="5" t="s">
         <v>14</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="I30" s="5"/>
-    </row>
-    <row r="31" spans="1:9" ht="63" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="F31" s="5" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="G31" s="5" t="s">
         <v>14</v>
@@ -1299,10 +1419,11 @@
       <c r="H31" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" ht="63" x14ac:dyDescent="0.25">
+      <c r="I31" s="5"/>
+    </row>
+    <row r="32" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="F32" s="5" t="s">
-        <v>23</v>
+        <v>62</v>
       </c>
       <c r="G32" s="5" t="s">
         <v>14</v>
@@ -1311,10 +1432,24 @@
         <v>63</v>
       </c>
     </row>
+    <row r="33" spans="6:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="F33" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="F2:H32">
-    <sortCondition ref="H2:H32"/>
+  <sortState ref="F3:H33">
+    <sortCondition ref="H3:H33"/>
   </sortState>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">

</xml_diff>